<commit_message>
added some stuff, can alsmost load a picture
</commit_message>
<xml_diff>
--- a/Planning & Group contract/ProjectPlan.xlsx
+++ b/Planning & Group contract/ProjectPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s225183_dtu_dk/Documents/Bachelor/IOTunderwater/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s225183_dtu_dk/Documents/Bachelor/IOTunderwater/Planning &amp; Group contract/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C8210D73-A987-F948-A249-6C8C59EA7407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{090DB292-7A62-4F7D-892A-4638EB1A5F91}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="13_ncr:1_{C8210D73-A987-F948-A249-6C8C59EA7407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E98B568C-5500-4E2F-92A8-4AE154096897}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34408076-A67B-844C-A01F-177E0C9C8862}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{34408076-A67B-844C-A01F-177E0C9C8862}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,89 +35,44 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={3999C0C1-207C-2B45-A4B1-43A190DC77A1}</author>
-    <author>tc={AF5FD766-F181-0448-A6DD-44B4229F8E73}</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{3999C0C1-207C-2B45-A4B1-43A190DC77A1}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Transmitter side:
-- RS-232 cable to connect 
-input source to:
-- Fucntion/Wave generator 
-- Underwater Speaker (Using BNC adapter)
-Receiver side:
-- hydrophone
-- loging device - oscilloscope or sound card
-- maybe an amplifier
-</t>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="1" shapeId="0" xr:uid="{AF5FD766-F181-0448-A6DD-44B4229F8E73}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Transmitter side:
-- RS-232 cable to connect 
-input source to:
-- Fucntion/Wave generator 
-- Underwater Speaker (Using BNC adapter)
-Receiver side:
-- hydrophone
-- loging device - oscilloscope or sound card
-- maybe an amplifier
-</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Uge </t>
+    <t>Activities / Week</t>
   </si>
   <si>
-    <t>Test equipment</t>
+    <t>Receive equipment</t>
   </si>
   <si>
-    <t>Document equipment</t>
+    <t>Optimize data transfer (both pre- and post processing)</t>
   </si>
   <si>
-    <t xml:space="preserve">Recieve equipment. </t>
+    <t>Write report</t>
   </si>
   <si>
-    <t>understand equipment in regards to usage</t>
+    <t>Understand, test and document equipment in regards to usage</t>
   </si>
   <si>
-    <t>Make test setup where we can transmit and recieve some signal with internal modulation and display osciliscope</t>
+    <t>Make test setup in a larger test area, such as the pool at dtu.</t>
   </si>
   <si>
-    <t>API til waveform generator. Implement necessary commands.Or find API that already can do this.</t>
+    <t xml:space="preserve">Transmit and recieve sinus wave in office setup </t>
   </si>
   <si>
-    <t>Send the value 42</t>
+    <t>Create API to signal generator in order to modulate carrier frequency with our own data</t>
   </si>
   <si>
-    <t>få mathias kniv ide til at virke:)</t>
+    <t>Transmit and recieve our own data in office setup</t>
   </si>
   <si>
-    <t>Audio conversion (.wav file) to array</t>
+    <t xml:space="preserve">Substitute components in the setup with cheaper and less power demanding components. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,16 +95,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -157,19 +163,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,9 +237,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Mathias Rohde Markvardsen" id="{A6F9BE36-2021-8D4D-9FCC-21C2078BF30C}" userId="S::mathias.markvardsen@epfl.ch::fd434c0a-1e8a-4400-babb-e3626cd7a92c" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,164 +555,737 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B2" dT="2025-02-12T13:39:48.99" personId="{A6F9BE36-2021-8D4D-9FCC-21C2078BF30C}" id="{3999C0C1-207C-2B45-A4B1-43A190DC77A1}">
-    <text xml:space="preserve">Transmitter side:
-- RS-232 cable to connect 
-input source to:
-- Fucntion/Wave generator 
-- Underwater Speaker (Using BNC adapter)
-Receiver side:
-- hydrophone
-- loging device - oscilloscope or sound card
-- maybe an amplifier
-</text>
-  </threadedComment>
-  <threadedComment ref="C2" dT="2025-02-12T13:39:48.99" personId="{A6F9BE36-2021-8D4D-9FCC-21C2078BF30C}" id="{AF5FD766-F181-0448-A6DD-44B4229F8E73}">
-    <text xml:space="preserve">Transmitter side:
-- RS-232 cable to connect 
-input source to:
-- Fucntion/Wave generator 
-- Underwater Speaker (Using BNC adapter)
-Receiver side:
-- hydrophone
-- loging device - oscilloscope or sound card
-- maybe an amplifier
-</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3809D6-D687-904C-BD08-E27870F364F3}">
-  <dimension ref="A1:P10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE3809D6-D687-904C-BD08-E27870F364F3}">
+  <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.69921875" customWidth="1"/>
-    <col min="3" max="3" width="19.19921875" customWidth="1"/>
+    <col min="1" max="1" width="29.3984375" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
+    <col min="3" max="3" width="11.3984375" customWidth="1"/>
     <col min="4" max="4" width="16.19921875" customWidth="1"/>
     <col min="5" max="5" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3">
+      <c r="B1" s="10">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="10">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="10">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="10">
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="10">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="10">
         <v>6</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="10">
         <v>7</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="10">
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="10">
         <v>9</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="10">
         <v>10</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="10">
         <v>11</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="10">
         <v>12</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N1" s="10">
         <v>13</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O1" s="10">
         <v>14</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P1" s="10">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:16" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="16"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="1:16" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="103.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="120" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="D8" s="1" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
-        <v>8</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="1"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="1"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="1"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="1"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="1"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="1"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="1"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="1"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="1"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="1"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="1"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="1"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="1"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="1"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="1"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="1"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="1"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="1"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="1"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="1"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="1"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="1"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="1"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="1"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="1"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="1"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="1"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="1"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="1"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="1"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="1"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="1"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="1"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="1"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="1"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="1"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="1"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="1"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="1"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="1"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="1"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="1"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="1"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="1"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>